<commit_message>
Fix spreadsheet error handling for no rows given
</commit_message>
<xml_diff>
--- a/docs/excelPlayground/3rows2rows.xlsx
+++ b/docs/excelPlayground/3rows2rows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\excelPlayground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0469D410-2FB4-44F8-A54A-0045F3FFE782}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA60AAA-3922-41E8-82A2-8F0E542760D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D76963E8-864B-457D-9DF5-20326BDCEA33}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>Count</t>
   </si>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6CFABE-B520-458B-807B-76EBB7A64E59}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3BADB4-F2E3-4D87-A259-6F969AA2D79C}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,9 +1105,7 @@
       <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
         <v>62</v>
       </c>

</xml_diff>